<commit_message>
feat: added vertex and triangle tracker
Added VertexCounter script which calculates the amount of vertices and triangles in the scene.

Updated the report document with an explanation of tessellation factor.
Updated the Data file with the amount of vertices and triangle from the first tests
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Year 2\TesselationTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E319B85E-D70A-41F1-BFFD-BDBEEB22E5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8052E586-CB76-4724-8844-F2333159CD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Test 1</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Average (FPS)</t>
   </si>
   <si>
-    <t>No tessellation</t>
-  </si>
-  <si>
     <t>Tessellation factor 4</t>
   </si>
   <si>
@@ -102,6 +99,15 @@
   </si>
   <si>
     <t>10x10 City; Seed 2; Min 3 Height; Max 5 Height</t>
+  </si>
+  <si>
+    <t>Tessellation factor 1 (no tesselation)</t>
+  </si>
+  <si>
+    <t>Triangle Count</t>
+  </si>
+  <si>
+    <t>Vertex Count</t>
   </si>
 </sst>
 </file>
@@ -143,9 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,21 +433,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -454,10 +463,16 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>99.74</v>
@@ -472,10 +487,16 @@
         <f>AVERAGE(B2:D2)</f>
         <v>99.236666666666665</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G2" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H2" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>95.07</v>
@@ -490,10 +511,16 @@
         <f t="shared" ref="E3:E18" si="0">AVERAGE(B3:D3)</f>
         <v>94.11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G3" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>94.57</v>
@@ -508,10 +535,16 @@
         <f t="shared" si="0"/>
         <v>93.686666666666667</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G4" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>90.85</v>
@@ -526,10 +559,16 @@
         <f t="shared" si="0"/>
         <v>90.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H5" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>91.52</v>
@@ -544,113 +583,191 @@
         <f t="shared" si="0"/>
         <v>90.726666666666674</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G6" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H6" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E8" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H8" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="E9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H9" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="E10" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H10" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="E11" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H11" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="E12" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H12" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="E13" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H13" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="E14" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H14" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="E15" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H15" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="E16" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H16" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="E17" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H17" s="2">
+        <v>8321936</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
       <c r="E18" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="2">
+        <v>5183814</v>
+      </c>
+      <c r="H18" s="2">
+        <v>8321936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>